<commit_message>
[ADD] all graphs and necessary files
</commit_message>
<xml_diff>
--- a/RdKit_Lipid_GEMA/final_results/iLB1027_lipid.xlsx
+++ b/RdKit_Lipid_GEMA/final_results/iLB1027_lipid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="89">
   <si>
     <t xml:space="preserve">True P</t>
   </si>
@@ -88,18 +88,27 @@
     <t xml:space="preserve">1-Phosphatidyl-1D-myo-inositol 3-phosphate</t>
   </si>
   <si>
+    <t xml:space="preserve">Phosphatidyl-4,5-BP</t>
+  </si>
+  <si>
     <t xml:space="preserve">PI-4,5-BP</t>
   </si>
   <si>
     <t xml:space="preserve">Phosphatidylinositol</t>
   </si>
   <si>
+    <t xml:space="preserve">Phosphatidyl-4-P</t>
+  </si>
+  <si>
     <t xml:space="preserve">PI-4-P</t>
   </si>
   <si>
     <t xml:space="preserve">1-Phosphatidyl-1D-myo-inositol 4,5-bisphosphate</t>
   </si>
   <si>
+    <t xml:space="preserve">Phosphatidyl-3-P</t>
+  </si>
+  <si>
     <t xml:space="preserve">PI-3-P</t>
   </si>
   <si>
@@ -145,7 +154,7 @@
     <t xml:space="preserve">Total</t>
   </si>
   <si>
-    <t xml:space="preserve">1–2-lysophos</t>
+    <t xml:space="preserve">lysophosphatidylcholine</t>
   </si>
   <si>
     <t xml:space="preserve">Hexadecanoate</t>
@@ -157,7 +166,7 @@
     <t xml:space="preserve">Monogalactosyldiacylglycerol</t>
   </si>
   <si>
-    <t xml:space="preserve">1-Acyl-sn-gly</t>
+    <t xml:space="preserve">1-Acyl-sn-glycero-3-PE</t>
   </si>
   <si>
     <t xml:space="preserve">Timnodonic acid C, n-3</t>
@@ -172,13 +181,10 @@
     <t xml:space="preserve">Diacylglyceryl-N,N,N-trimethyl-beta-alanine</t>
   </si>
   <si>
-    <t xml:space="preserve">1-monoacylgl</t>
-  </si>
-  <si>
     <t xml:space="preserve">1-monoacylglycerol</t>
   </si>
   <si>
-    <t xml:space="preserve">1–2-lysophosp</t>
+    <t xml:space="preserve">lysophosphatidylethanolamine</t>
   </si>
   <si>
     <t xml:space="preserve">Palmitoyl-CoA</t>
@@ -526,16 +532,16 @@
   <dimension ref="A1:S60"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P29" activeCellId="0" sqref="P29"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.46"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="12" min="12" style="1" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16381" style="1" width="9.14"/>
@@ -941,7 +947,7 @@
         <v>1</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N8" s="6" t="n">
         <v>16</v>
@@ -964,13 +970,13 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>16</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" s="6" t="n">
         <v>16</v>
@@ -995,7 +1001,7 @@
         <v>1</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="N9" s="6" t="n">
         <v>16</v>
@@ -1018,13 +1024,13 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>16</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E10" s="6" t="n">
         <v>16</v>
@@ -1049,7 +1055,7 @@
         <v>1</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="N10" s="6" t="n">
         <v>16</v>
@@ -1072,13 +1078,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>16</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E11" s="6" t="n">
         <v>6</v>
@@ -1103,7 +1109,7 @@
         <v>0.428571428571429</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="N11" s="6" t="n">
         <v>6</v>
@@ -1126,13 +1132,13 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>10</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E12" s="6" t="n">
         <v>5</v>
@@ -1157,7 +1163,7 @@
         <v>1</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N12" s="6" t="n">
         <v>5</v>
@@ -1180,13 +1186,13 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>9</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E13" s="6" t="n">
         <v>5</v>
@@ -1211,7 +1217,7 @@
         <v>0.714285714285714</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="N13" s="6" t="n">
         <v>5</v>
@@ -1234,13 +1240,13 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>8</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E14" s="6" t="n">
         <v>3</v>
@@ -1265,7 +1271,7 @@
         <v>1</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="N14" s="6" t="n">
         <v>3</v>
@@ -1288,13 +1294,13 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>7</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E15" s="6" t="n">
         <v>2</v>
@@ -1319,7 +1325,7 @@
         <v>1</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="N15" s="6" t="n">
         <v>2</v>
@@ -1342,13 +1348,13 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E16" s="6" t="n">
         <v>2</v>
@@ -1373,7 +1379,7 @@
         <v>0.333333333333333</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="N16" s="6" t="n">
         <v>2</v>
@@ -1396,13 +1402,13 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E17" s="6" t="n">
         <v>1</v>
@@ -1427,7 +1433,7 @@
         <v>0.666666666666667</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="N17" s="6" t="n">
         <v>1</v>
@@ -1450,13 +1456,13 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E18" s="3" t="n">
         <f aca="false">SUM(E2:E17)</f>
@@ -1480,7 +1486,7 @@
         <v>0.957281553398058</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="N18" s="6" t="n">
         <v>0</v>
@@ -1504,13 +1510,13 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>3</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="N19" s="6" t="n">
         <v>0</v>
@@ -1534,7 +1540,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>3</v>
@@ -1543,7 +1549,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="M20" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="N20" s="6" t="n">
         <v>0</v>
@@ -1567,7 +1573,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>3</v>
@@ -1576,7 +1582,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="M21" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N21" s="6" t="n">
         <v>0</v>
@@ -1600,14 +1606,14 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E22" s="1"/>
       <c r="M22" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="N22" s="6" t="n">
         <v>0</v>
@@ -1631,13 +1637,13 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>3</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="N23" s="6" t="n">
         <v>0</v>
@@ -1661,13 +1667,13 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>3</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="N24" s="6" t="n">
         <v>0</v>
@@ -1691,13 +1697,13 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>3</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="N25" s="3" t="n">
         <f aca="false">SUM(N2:N24)</f>
@@ -1723,7 +1729,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>3</v>
@@ -1731,7 +1737,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>2</v>
@@ -1742,7 +1748,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>2</v>
@@ -1753,7 +1759,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>2</v>
@@ -1763,7 +1769,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>2</v>
@@ -1773,7 +1779,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>2</v>
@@ -1781,7 +1787,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>2</v>
@@ -1789,7 +1795,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>2</v>
@@ -1797,7 +1803,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>2</v>
@@ -1805,7 +1811,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>2</v>
@@ -1813,7 +1819,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>2</v>
@@ -1821,7 +1827,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>2</v>
@@ -1829,7 +1835,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>2</v>
@@ -1837,7 +1843,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>2</v>
@@ -1845,7 +1851,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>2</v>
@@ -1853,7 +1859,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>2</v>
@@ -1861,7 +1867,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>2</v>
@@ -1869,7 +1875,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>2</v>
@@ -1877,7 +1883,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="11" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B44" s="1" t="n">
         <v>2</v>
@@ -1885,7 +1891,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>2</v>
@@ -1893,7 +1899,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B46" s="1" t="n">
         <v>2</v>
@@ -1901,7 +1907,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>2</v>
@@ -1909,7 +1915,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>2</v>
@@ -1917,7 +1923,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>2</v>
@@ -1925,7 +1931,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>2</v>
@@ -1933,7 +1939,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B51" s="1" t="n">
         <v>2</v>
@@ -1941,7 +1947,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B52" s="1" t="n">
         <v>1</v>
@@ -1949,7 +1955,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B53" s="1" t="n">
         <v>1</v>
@@ -1957,7 +1963,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B54" s="1" t="n">
         <v>1</v>
@@ -1965,7 +1971,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B55" s="1" t="n">
         <v>1</v>
@@ -1973,7 +1979,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B56" s="1" t="n">
         <v>1</v>
@@ -1981,7 +1987,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="11" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B57" s="1" t="n">
         <v>1</v>
@@ -1989,7 +1995,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="11" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B58" s="1" t="n">
         <v>1</v>
@@ -1997,7 +2003,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B59" s="1" t="n">
         <v>1</v>

</xml_diff>